<commit_message>
Changed team answer dto
</commit_message>
<xml_diff>
--- a/UML/API endpoints.xlsx
+++ b/UML/API endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidas\Dropbox\STUDIJOS\Bakalauras\Mindfights\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD59290-3284-43E6-A742-0FEDBE7140EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ECDFEA-EB04-4E84-A556-884448CB9690}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{5B70543C-F736-4368-AC7C-F0DABC0D76F8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="219">
   <si>
     <t>Type</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>UpdateUserActiveStatus</t>
   </si>
 </sst>
 </file>
@@ -2978,10 +2981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188D6225-717C-45AD-89EE-E82E7237B7D9}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,25 +3421,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>208</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>217</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>217</v>
@@ -3458,45 +3458,56 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>217</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>217</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>217</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="C65" s="27" t="s">
         <v>217</v>
       </c>
       <c r="D65" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D66" s="26" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>